<commit_message>
Todas las ventanas completamente funcionales
</commit_message>
<xml_diff>
--- a/Plantillas/Solicitud_Pago.xlsx
+++ b/Plantillas/Solicitud_Pago.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>SOLICITUD DE PAGO</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>Fecha límite de pago:</t>
-  </si>
-  <si>
-    <t>Pronto Pago</t>
   </si>
   <si>
     <t>Número(s)  de factura (s)</t>
@@ -282,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -403,6 +400,17 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -420,7 +428,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -469,28 +477,153 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="9" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
@@ -498,149 +631,33 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="7" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="9" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -681,7 +698,7 @@
         <xdr:cNvPr id="2" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1006821E-05CB-407A-8E00-6B6DE0C6D665}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1006821E-05CB-407A-8E00-6B6DE0C6D665}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1008,8 +1025,8 @@
   </sheetPr>
   <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S31" sqref="S31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1030,71 +1047,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="64" t="s">
+      <c r="A1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="66"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:14" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="59"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="69"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
     </row>
     <row r="3" spans="1:14" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="69"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="39"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="61"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="63"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="70"/>
-      <c r="H4" s="71">
+      <c r="G4" s="40"/>
+      <c r="H4" s="41">
         <v>45505</v>
       </c>
-      <c r="I4" s="70"/>
-      <c r="J4" s="72" t="s">
+      <c r="I4" s="40"/>
+      <c r="J4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="73"/>
+      <c r="K4" s="43"/>
       <c r="L4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1104,37 +1121,37 @@
       <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="74"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="33"/>
-      <c r="H8" s="27" t="s">
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="H8" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
     </row>
     <row r="9" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="6"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="77"/>
-      <c r="K9" s="77"/>
-      <c r="L9" s="77"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
     </row>
     <row r="10" spans="1:14" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="7"/>
@@ -1148,30 +1165,30 @@
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
     </row>
     <row r="12" spans="1:14" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
     </row>
     <row r="13" spans="1:14" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="8"/>
@@ -1179,30 +1196,30 @@
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="33"/>
-      <c r="G14" s="47" t="s">
+      <c r="D14" s="46"/>
+      <c r="E14" s="47"/>
+      <c r="G14" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="48"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
     </row>
     <row r="15" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="51"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="61"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
     </row>
     <row r="16" spans="1:14" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="9"/>
@@ -1218,32 +1235,32 @@
       <c r="N16" s="13"/>
     </row>
     <row r="17" spans="3:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="33"/>
-      <c r="G17" s="54" t="s">
+      <c r="D17" s="46"/>
+      <c r="E17" s="47"/>
+      <c r="G17" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="55"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
     </row>
     <row r="18" spans="3:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
-      <c r="G18" s="79"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="78"/>
-      <c r="J18" s="78"/>
-      <c r="K18" s="78"/>
-      <c r="L18" s="78"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="68"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="66"/>
     </row>
     <row r="19" spans="3:23" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" s="7"/>
@@ -1253,21 +1270,21 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="3:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="33"/>
-      <c r="G20" s="27" t="s">
+      <c r="D20" s="46"/>
+      <c r="E20" s="47"/>
+      <c r="G20" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="27"/>
+      <c r="H20" s="46"/>
       <c r="I20" s="8"/>
-      <c r="J20" s="41" t="s">
+      <c r="J20" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
     </row>
     <row r="21" spans="3:23" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="7" t="s">
@@ -1284,15 +1301,15 @@
       <c r="L21" s="15"/>
     </row>
     <row r="22" spans="3:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="38"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="51"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="44"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="52"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
     </row>
     <row r="23" spans="3:23" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="7"/>
@@ -1307,57 +1324,57 @@
       <c r="L23" s="7"/>
     </row>
     <row r="24" spans="3:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="34"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="S24" s="30"/>
-      <c r="T24" s="31"/>
-      <c r="U24" s="31"/>
-      <c r="V24" s="31"/>
-      <c r="W24" s="31"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="S24" s="71"/>
+      <c r="T24" s="72"/>
+      <c r="U24" s="72"/>
+      <c r="V24" s="72"/>
+      <c r="W24" s="72"/>
     </row>
     <row r="25" spans="3:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="S25" s="31"/>
-      <c r="T25" s="31"/>
-      <c r="U25" s="31"/>
-      <c r="V25" s="31"/>
-      <c r="W25" s="31"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="S25" s="72"/>
+      <c r="T25" s="72"/>
+      <c r="U25" s="72"/>
+      <c r="V25" s="72"/>
+      <c r="W25" s="72"/>
     </row>
     <row r="26" spans="3:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="S26" s="31"/>
-      <c r="T26" s="31"/>
-      <c r="U26" s="31"/>
-      <c r="V26" s="31"/>
-      <c r="W26" s="31"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="73"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="73"/>
+      <c r="L26" s="73"/>
+      <c r="S26" s="72"/>
+      <c r="T26" s="72"/>
+      <c r="U26" s="72"/>
+      <c r="V26" s="72"/>
+      <c r="W26" s="72"/>
     </row>
     <row r="27" spans="3:23" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C27" s="7"/>
@@ -1370,48 +1387,45 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
-      <c r="S27" s="31"/>
-      <c r="T27" s="31"/>
-      <c r="U27" s="31"/>
-      <c r="V27" s="31"/>
-      <c r="W27" s="31"/>
+      <c r="S27" s="72"/>
+      <c r="T27" s="72"/>
+      <c r="U27" s="72"/>
+      <c r="V27" s="72"/>
+      <c r="W27" s="72"/>
     </row>
     <row r="28" spans="3:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="33"/>
-      <c r="G28" s="27" t="s">
+      <c r="D28" s="46"/>
+      <c r="E28" s="47"/>
+      <c r="G28" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="S28" s="31"/>
-      <c r="T28" s="31"/>
-      <c r="U28" s="31"/>
-      <c r="V28" s="31"/>
-      <c r="W28" s="31"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
+      <c r="S28" s="72"/>
+      <c r="T28" s="72"/>
+      <c r="U28" s="72"/>
+      <c r="V28" s="72"/>
+      <c r="W28" s="72"/>
     </row>
     <row r="29" spans="3:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="36">
+      <c r="C29" s="74">
         <f>C9</f>
         <v>0</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="37"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="82"/>
+      <c r="J29" s="82"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="83"/>
       <c r="R29" s="13"/>
       <c r="S29" s="13"/>
       <c r="T29" s="13"/>
@@ -1448,19 +1462,19 @@
       <c r="U31" s="13"/>
     </row>
     <row r="32" spans="3:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="55"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="H32" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="H32" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
       <c r="R32" s="13"/>
       <c r="S32" s="16"/>
       <c r="T32" s="13"/>
@@ -1471,27 +1485,27 @@
       <c r="D33" s="8"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
-      <c r="H33" s="80"/>
-      <c r="I33" s="80"/>
-      <c r="J33" s="80"/>
-      <c r="K33" s="80"/>
-      <c r="L33" s="80"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
       <c r="R33" s="13"/>
       <c r="S33" s="16"/>
       <c r="T33" s="13"/>
       <c r="U33" s="13"/>
     </row>
     <row r="34" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
       <c r="G34" s="7"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
+      <c r="H34" s="80"/>
+      <c r="I34" s="80"/>
+      <c r="J34" s="80"/>
+      <c r="K34" s="80"/>
+      <c r="L34" s="80"/>
       <c r="R34" s="13"/>
       <c r="S34" s="17"/>
       <c r="T34" s="13"/>
@@ -1503,85 +1517,85 @@
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
       <c r="R35" s="13"/>
       <c r="S35" s="17"/>
       <c r="T35" s="13"/>
       <c r="U35" s="13"/>
     </row>
     <row r="36" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="7"/>
+      <c r="H36" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="7"/>
-      <c r="H36" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="27"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="46"/>
       <c r="R36" s="13"/>
       <c r="S36" s="17"/>
       <c r="T36" s="13"/>
       <c r="U36" s="13"/>
     </row>
     <row r="37" spans="2:21" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="78" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="78"/>
+      <c r="E37" s="79"/>
+      <c r="F37" s="79"/>
+      <c r="H37" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="D37" s="28"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="H37" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
+      <c r="I37" s="79"/>
+      <c r="J37" s="79"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="79"/>
       <c r="R37" s="13"/>
       <c r="S37" s="13"/>
       <c r="T37" s="13"/>
       <c r="U37" s="13"/>
     </row>
     <row r="38" spans="2:21" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="79"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="79"/>
+      <c r="H38" s="79"/>
+      <c r="I38" s="79"/>
+      <c r="J38" s="79"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="79"/>
     </row>
     <row r="39" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
+      <c r="C39" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="75"/>
+      <c r="E39" s="75"/>
       <c r="F39" s="9"/>
-      <c r="H39" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
+      <c r="H39" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="I39" s="75"/>
+      <c r="J39" s="75"/>
+      <c r="K39" s="75"/>
+      <c r="L39" s="75"/>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
       <c r="F40" s="20"/>
       <c r="N40" s="21">
         <v>45642</v>
@@ -1595,18 +1609,23 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="C12:L12"/>
-    <mergeCell ref="A1:C4"/>
-    <mergeCell ref="D1:L3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="C11:L11"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="H36:L36"/>
+    <mergeCell ref="C37:F38"/>
+    <mergeCell ref="H37:L38"/>
+    <mergeCell ref="H34:L35"/>
+    <mergeCell ref="S24:W28"/>
+    <mergeCell ref="C25:L26"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="G28:L28"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="H29:L29"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="J22:L22"/>
@@ -1622,23 +1641,18 @@
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="J20:L20"/>
-    <mergeCell ref="S24:W28"/>
-    <mergeCell ref="C25:L26"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="G28:L28"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="G29:L29"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="H39:L39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="H36:L36"/>
-    <mergeCell ref="C37:F38"/>
-    <mergeCell ref="H37:L38"/>
-    <mergeCell ref="H34:L35"/>
+    <mergeCell ref="C12:L12"/>
+    <mergeCell ref="A1:C4"/>
+    <mergeCell ref="D1:L3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="C11:L11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>